<commit_message>
odd part 3 added
</commit_message>
<xml_diff>
--- a/Proje Görev Paylaşım.xlsx
+++ b/Proje Görev Paylaşım.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CEAD78-47F2-46A2-8C49-1A4FE24C72AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774DB321-1432-4E4A-8CBC-3C57197A49DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
   <si>
     <t>Front-End</t>
   </si>
@@ -306,7 +306,7 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3"/>
@@ -321,6 +321,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="%40 - Vurgu3" xfId="6" builtinId="39"/>
@@ -613,7 +614,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -776,6 +777,9 @@
       <c r="B11" s="8" t="s">
         <v>17</v>
       </c>
+      <c r="C11" s="12" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">

</xml_diff>